<commit_message>
Documented Utils and Program
</commit_message>
<xml_diff>
--- a/RF_ASM/Documentation/Reference/InstructionList.xlsx
+++ b/RF_ASM/Documentation/Reference/InstructionList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\VisualStudio C#\RedFox Assembly\RF_ASM\RF_ASM\Documentation\Reference\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8e6494fb9429eb6/Desktop/Programming/RF_ASM/RF_ASM/Documentation/Reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623D4B9F-8A06-4B03-B2EB-9B7362BBA53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{623D4B9F-8A06-4B03-B2EB-9B7362BBA53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC950906-2773-4C82-99E1-589E0F853FA9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BBCE24B3-AA34-466A-BF03-56E58F9E96A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BBCE24B3-AA34-466A-BF03-56E58F9E96A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -572,16 +572,16 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="67.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="73.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -603,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -614,7 +614,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -625,7 +625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -636,7 +636,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -647,7 +647,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -658,7 +658,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -669,7 +669,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -680,7 +680,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -691,7 +691,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -702,7 +702,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -713,7 +713,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -724,7 +724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
@@ -735,7 +735,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
@@ -746,7 +746,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -757,7 +757,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>